<commit_message>
Add A55E49 variants and update emissions bounds for the rest
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65-EA.xlsx
+++ b/SuppXLS/Scen_SYS_ZeroCO2_CAP21-A25E65-EA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9A1619-31A5-442E-B5ED-C3E0E4F6937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A8F806-1E0B-463E-94F4-9F22496BE373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -1903,7 +1903,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,34 +2069,34 @@
         <v>33792</v>
       </c>
       <c r="D7" s="16">
-        <v>31606</v>
+        <v>30962</v>
       </c>
       <c r="E7" s="16">
-        <v>29562</v>
+        <v>28369</v>
       </c>
       <c r="F7" s="16">
-        <v>27650</v>
+        <v>25994</v>
       </c>
       <c r="G7" s="16">
-        <v>25861</v>
+        <v>23817</v>
       </c>
       <c r="H7" s="16">
-        <v>24189</v>
+        <v>21823</v>
       </c>
       <c r="I7" s="16">
-        <v>22624</v>
+        <v>19995</v>
       </c>
       <c r="J7" s="16">
-        <v>21161</v>
+        <v>18321</v>
       </c>
       <c r="K7" s="16">
-        <v>19792</v>
+        <v>16787</v>
       </c>
       <c r="L7" s="16">
-        <v>18512</v>
+        <v>15381</v>
       </c>
       <c r="M7" s="16">
-        <v>12482</v>
+        <v>14093</v>
       </c>
       <c r="N7" s="16">
         <v>0</v>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
-        <v>31606</v>
+        <v>30962</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="J11" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
-        <v>29562</v>
+        <v>28369</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="J13" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
-        <v>27650</v>
+        <v>25994</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2808,7 +2808,7 @@
       </c>
       <c r="J15" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
-        <v>25861</v>
+        <v>23817</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="J17" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
-        <v>24189</v>
+        <v>21823</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="J19" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
-        <v>22624</v>
+        <v>19995</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
@@ -2949,7 +2949,7 @@
       </c>
       <c r="J21" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
-        <v>21161</v>
+        <v>18321</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="J23" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
-        <v>19792</v>
+        <v>16787</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
       </c>
       <c r="J25" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
-        <v>18512</v>
+        <v>15381</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="J27" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
-        <v>12482</v>
+        <v>14093</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="J9" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
-        <v>31606</v>
+        <v>30962</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="J11" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
-        <v>29562</v>
+        <v>28369</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="J13" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
-        <v>27650</v>
+        <v>25994</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="J15" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
-        <v>25861</v>
+        <v>23817</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="J17" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
-        <v>24189</v>
+        <v>21823</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="J19" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
-        <v>22624</v>
+        <v>19995</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="J21" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
-        <v>21161</v>
+        <v>18321</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="J23" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
-        <v>19792</v>
+        <v>16787</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
       </c>
       <c r="J25" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
-        <v>18512</v>
+        <v>15381</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="J27" s="8">
         <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
-        <v>12482</v>
+        <v>14093</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>